<commit_message>
add new details about otuput table
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaneff/Documents/covid-ensemble/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C96ACCC-4A16-3D44-B4BB-61EFE73B2F22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D01A42A-A41C-2A43-9A8F-E511952ED339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="6860" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
+    <workbookView xWindow="3200" yWindow="1960" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>Table name</t>
   </si>
@@ -229,13 +229,58 @@
   </si>
   <si>
     <t>A definition of each model output, used to ensure alignment of model outputs across models</t>
+  </si>
+  <si>
+    <t>any integer that corresponds to a unique output_id specified in the outputs table</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>One of:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cumulative fatalities
+cumulative cases
+ICU beds per day
+ventilators per day
+hospital admissions per day
+ICU admissions per day
+fatalities per day
+(additional outputs to be added, in progress)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,6 +292,22 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -605,7 +666,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,8 +752,8 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,10 +1013,10 @@
         <v>51</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -966,7 +1027,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -1025,7 +1086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1036,7 +1097,7 @@
         <v>53</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
restructure files for consistency across model_runs subdirectory
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaneff/Documents/covid-ensemble/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D01A42A-A41C-2A43-9A8F-E511952ED339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2815DCCD-CC84-4648-9728-1A4187460052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="1960" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
+    <workbookView xWindow="8580" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>Table name</t>
   </si>
@@ -274,6 +274,12 @@
 fatalities per day
 (additional outputs to be added, in progress)</t>
     </r>
+  </si>
+  <si>
+    <t>run_name</t>
+  </si>
+  <si>
+    <t>A brief description of the model run used to generate legends in plots</t>
   </si>
 </sst>
 </file>
@@ -749,11 +755,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF9E1D9-8E87-7B41-8BD2-4E4EA8040297}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,18 +882,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -895,222 +901,250 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="151" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
       <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Imperial College London model outputs from 4/7/2020
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaneff/Documents/covid-ensemble/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2815DCCD-CC84-4648-9728-1A4187460052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D57D65-0806-FE4E-AB02-DEEEE2609C0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
+    <workbookView xWindow="5560" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>The name of each model output (e.g., cumulative caseload)</t>
-  </si>
-  <si>
-    <t>If the model output is associated with a specified date, the specified date of that output (e.g., cumulative caseload as of June 10, 2020). Otherwise this field should be NA</t>
   </si>
   <si>
     <t>If the model output is associated with a specified location, the specified location of that output (e.g., cumulative caseload as of June 10, 2020 in California). Otherwise this field should be NA</t>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>A brief description of the model run used to generate legends in plots</t>
+  </si>
+  <si>
+    <t>If the model output is associated with a specified date, the specified date of that output (e.g., cumulative caseload as of June 10, 2020). If data are reported per week or per month, date should be specified as the end date of the given week or month. Please note that weeks are defined as beginning on Monday and ending on Sunday, to align with available Imperial College London projections.</t>
   </si>
 </sst>
 </file>
@@ -739,13 +739,13 @@
     </row>
     <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -758,8 +758,8 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -887,10 +887,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>28</v>
@@ -1019,7 +1019,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>33</v>
@@ -1047,7 +1047,7 @@
         <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
@@ -1061,7 +1061,7 @@
         <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -1072,7 +1072,7 @@
         <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>37</v>
@@ -1086,7 +1086,7 @@
         <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>28</v>
@@ -1100,21 +1100,21 @@
         <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>20</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="26" spans="1:4" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
         <v>52</v>
@@ -1131,18 +1131,18 @@
         <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
add some additional model documentation in the models table
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaneff/Documents/covid-ensemble/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D57D65-0806-FE4E-AB02-DEEEE2609C0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42711540-FECE-9748-9A36-903DF2462001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
+    <workbookView xWindow="14500" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Table name</t>
   </si>
@@ -280,6 +280,21 @@
   </si>
   <si>
     <t>If the model output is associated with a specified date, the specified date of that output (e.g., cumulative caseload as of June 10, 2020). If data are reported per week or per month, date should be specified as the end date of the given week or month. Please note that weeks are defined as beginning on Monday and ending on Sunday, to align with available Imperial College London projections.</t>
+  </si>
+  <si>
+    <t>geographic_resolution_US_state</t>
+  </si>
+  <si>
+    <t>geographic_resolution_country</t>
+  </si>
+  <si>
+    <t>Whether or not the model currently produced projections for one or more US states (e.g., are results available at the state level in the US?)</t>
+  </si>
+  <si>
+    <t>Whether or not the model currently produced projections for one or more countries (e.g., are results available at the country level, in the US or internationally?)</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -755,11 +770,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF9E1D9-8E87-7B41-8BD2-4E4EA8040297}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,46 +869,46 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -901,27 +916,27 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -929,222 +944,250 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
       <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="151" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>58</v>
       </c>
       <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add notes about unclear Imperial College London dates
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaneff/Documents/covid-ensemble/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42711540-FECE-9748-9A36-903DF2462001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D32E833-C76D-AD4D-B3AF-7BE1AB668658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14500" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
+    <workbookView xWindow="6940" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -279,9 +279,6 @@
     <t>A brief description of the model run used to generate legends in plots</t>
   </si>
   <si>
-    <t>If the model output is associated with a specified date, the specified date of that output (e.g., cumulative caseload as of June 10, 2020). If data are reported per week or per month, date should be specified as the end date of the given week or month. Please note that weeks are defined as beginning on Monday and ending on Sunday, to align with available Imperial College London projections.</t>
-  </si>
-  <si>
     <t>geographic_resolution_US_state</t>
   </si>
   <si>
@@ -295,6 +292,9 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>If the model output is associated with a specified date, the specified date of that output (e.g., cumulative caseload as of June 10, 2020). If data are reported per week or per month, date should be specified as the end date of the given week or month. Please note that weeks are defined as beginning on Sunday and ending on Saturday, to align with available Imperial College London projections. Note that weeks are currently (as of 4/8/20) handled inconsistently between Imperial College data export and documentation, so this may be updated moving forwards.</t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,13 +874,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
@@ -888,13 +888,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52" customHeight="1" x14ac:dyDescent="0.2">
@@ -1115,7 +1115,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
add new location information including ISO codes, make corresponding updates to data dictionary
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaneff/Documents/covid-ensemble/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77274BA6-F569-3F4A-98C3-45666AF5F710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5911F661-E502-5F4C-8021-C85958F0FC9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
+    <workbookView xWindow="2980" yWindow="1420" windowWidth="28040" windowHeight="17440" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
   <si>
     <t>Table name</t>
   </si>
@@ -308,12 +308,145 @@
   <si>
     <t>A brief description of the intended use of the model, as defined by the model developer. Whenever possible, this text is taken verbatim from the model developer's documentation or public-facing site</t>
   </si>
+  <si>
+    <t>locations</t>
+  </si>
+  <si>
+    <t>Table of all locations for which model outputs from any model are currently available</t>
+  </si>
+  <si>
+    <t>One row per unique location (includes cities, states/provinces, regions, cities, and other administrative areas)</t>
+  </si>
+  <si>
+    <t>iso2</t>
+  </si>
+  <si>
+    <t>iso3</t>
+  </si>
+  <si>
+    <t>location_type</t>
+  </si>
+  <si>
+    <t>area_level</t>
+  </si>
+  <si>
+    <t>location_name</t>
+  </si>
+  <si>
+    <t>abbreviation</t>
+  </si>
+  <si>
+    <t>FIPS</t>
+  </si>
+  <si>
+    <t>The unique ISO alpha-2 code of the country in which the location is located (or if the location is a country, the ISO code of that country). Codes based on ISO 3166 international standard, additional details available online: https://www.iban.com/country-codes</t>
+  </si>
+  <si>
+    <t>The unique ISO alpha-3 code of the country in which the location is located (or if the location is a country, the ISO code of that country). Codes based on ISO 3166 international standard, additional details available online: https://www.iban.com/country-codes</t>
+  </si>
+  <si>
+    <t>any text field (with under 3 characters)</t>
+  </si>
+  <si>
+    <t>any text field (with under 4 characters)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>One of:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Country
+Province/state
+Other
+(additional types, in progress)</t>
+    </r>
+  </si>
+  <si>
+    <t>The type of location or administrative area. Locations are specified as countries or province/states to ensure alignment to the extent possible with the existing format of data made available through the Johns Hopkins COVID-19 dashboard.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>One of:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Country
+Intermediate
+Local</t>
+    </r>
+  </si>
+  <si>
+    <t>The level of geopolitical organization of the location. These data are coded in accordance with the definitions provided by the Georgetown University IHR Costing Tool to ensure alignment to the extent possible. Intermediate areas are defined as large geopolitical units under the central government and may include states, regions, provinces, or territories. Local areas are smaller geopolitical units under the central government and may include cities or counties.</t>
+  </si>
+  <si>
+    <t>A unique name of the location</t>
+  </si>
+  <si>
+    <t>any text field</t>
+  </si>
+  <si>
+    <t>Where relevant, a non-ISO abbreviation of the location (e.g., US state abbreviation)</t>
+  </si>
+  <si>
+    <t>For US states and counties, the unique  Federal Information Processing Standard Publication (FIPS) code of the state or county</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,6 +478,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -372,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -380,6 +519,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -695,21 +837,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA005356-F3EE-BD4C-AF48-3C06F2B5C2C9}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="58" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -720,7 +862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="56" customHeight="1">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -731,7 +873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="68">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -742,7 +884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="63" customHeight="1">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -753,7 +895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="75" customHeight="1">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -764,7 +906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="68">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -773,6 +915,17 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -782,14 +935,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF9E1D9-8E87-7B41-8BD2-4E4EA8040297}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
@@ -797,7 +950,7 @@
     <col min="4" max="4" width="44.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="20">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -811,7 +964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="48" customHeight="1">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -825,7 +978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="43" customHeight="1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -839,7 +992,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="40" customHeight="1">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -853,7 +1006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="53" customHeight="1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -867,7 +1020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="53" customHeight="1">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -881,7 +1034,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="152" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="152" customHeight="1">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -895,7 +1048,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="56" customHeight="1">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -909,7 +1062,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="56" customHeight="1">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -923,7 +1076,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="56" customHeight="1">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -937,7 +1090,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="52" customHeight="1">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -951,7 +1104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="50" customHeight="1">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -965,7 +1118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="50" customHeight="1">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -979,7 +1132,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="50" customHeight="1">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -993,7 +1146,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="71" customHeight="1">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1007,7 +1160,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="50" customHeight="1">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1021,7 +1174,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="50" customHeight="1">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="45" customHeight="1">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="44" customHeight="1">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="59" customHeight="1">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1077,7 +1230,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="51">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1091,7 +1244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="53" customHeight="1">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +1258,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="58" customHeight="1">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1119,7 +1272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="55" customHeight="1">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1133,7 +1286,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="146" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="146" customHeight="1">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1300,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="50" customHeight="1">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1161,7 +1314,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="56" customHeight="1">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1175,7 +1328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="48" customHeight="1">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1189,7 +1342,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="35" customHeight="1">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1203,7 +1356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="151" customHeight="1">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1217,7 +1370,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="50" customHeight="1">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1231,7 +1384,96 @@
         <v>28</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="69" customHeight="1">
+      <c r="A32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="65" customHeight="1">
+      <c r="A33" s="4"/>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="85">
+      <c r="A34" s="4"/>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="136">
+      <c r="A35" s="4"/>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17">
+      <c r="A36" s="4"/>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="34">
+      <c r="A37" s="4"/>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="34">
+      <c r="A38" s="4"/>
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A32:A38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
get Shaman model (most reost recent run only) integrated
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seaneff/Documents/covid-ensemble/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5911F661-E502-5F4C-8021-C85958F0FC9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB104BCE-9477-714E-B0A7-73F0395F08B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="1420" windowWidth="28040" windowHeight="17440" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
+    <workbookView xWindow="9180" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AA0FE2F5-2A8E-324E-81F6-DC3A81D95E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="108">
   <si>
     <t>Table name</t>
   </si>
@@ -440,6 +440,30 @@
   </si>
   <si>
     <t>For US states and counties, the unique  Federal Information Processing Standard Publication (FIPS) code of the state or county</t>
+  </si>
+  <si>
+    <t>key_assumptions</t>
+  </si>
+  <si>
+    <t>A brief description, in writing, of key assumptions used in the model run</t>
+  </si>
+  <si>
+    <t>compare_across_models</t>
+  </si>
+  <si>
+    <t>compare_over_time</t>
+  </si>
+  <si>
+    <t>compare_across_assumptions</t>
+  </si>
+  <si>
+    <t>This information is only used to power the Shiny app used to visualize these data. The field indicates whether a given run of the model is eligible for comparison across models. This will be set to "FALSE", for instance, in cases where the model assumes no underlying intervention and thus is not directly comparable to other models that assume sustained social distancing.</t>
+  </si>
+  <si>
+    <t>This information is only used to power the Shiny app used to visualize these data. The field indicates whether a given run of the model is eligible for comparison with itself (e.g., prior versions of the same model) over time.</t>
+  </si>
+  <si>
+    <t>This information is only used to power the Shiny app used to visualize these data. The field indicates whether a given run of the model is eligible for comparison with itself (e.g., other versions of model model using different assumptions, for example assuming different levels of social distancing).</t>
   </si>
 </sst>
 </file>
@@ -839,7 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA005356-F3EE-BD4C-AF48-3C06F2B5C2C9}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -935,11 +959,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF9E1D9-8E87-7B41-8BD2-4E4EA8040297}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1137,342 +1161,398 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="71" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="50" customHeight="1">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="50" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="71" customHeight="1">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="106" customHeight="1">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="71" customHeight="1">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="92" customHeight="1">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="50" customHeight="1">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="50" customHeight="1">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45" customHeight="1">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="44" customHeight="1">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="59" customHeight="1">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="51">
+    <row r="21" spans="1:4" ht="50" customHeight="1">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="53" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" customHeight="1">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="44" customHeight="1">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="59" customHeight="1">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="53" customHeight="1">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="58" customHeight="1">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="55" customHeight="1">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="146" customHeight="1">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="50" customHeight="1">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="56" customHeight="1">
+    <row r="27" spans="1:4" ht="58" customHeight="1">
       <c r="A27" t="s">
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="48" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="55" customHeight="1">
       <c r="A28" t="s">
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="146" customHeight="1">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="50" customHeight="1">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="56" customHeight="1">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="48" customHeight="1">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="35" customHeight="1">
-      <c r="A29" t="s">
+    <row r="33" spans="1:4" ht="35" customHeight="1">
+      <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B33" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="151" customHeight="1">
-      <c r="A30" t="s">
+    <row r="34" spans="1:4" ht="151" customHeight="1">
+      <c r="A34" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B34" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="50" customHeight="1">
-      <c r="A31" t="s">
+    <row r="35" spans="1:4" ht="50" customHeight="1">
+      <c r="A35" t="s">
         <v>57</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B35" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="69" customHeight="1">
-      <c r="A32" s="4" t="s">
+    <row r="36" spans="1:4" ht="69" customHeight="1">
+      <c r="A36" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B36" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="65" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="85">
-      <c r="A34" s="4"/>
-      <c r="B34" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="136">
-      <c r="A35" s="4"/>
-      <c r="B35" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17">
-      <c r="A36" s="4"/>
-      <c r="B36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="34">
+    <row r="37" spans="1:4" ht="65" customHeight="1">
       <c r="A37" s="4"/>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="34">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="85">
       <c r="A38" s="4"/>
       <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="136">
+      <c r="A39" s="4"/>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17">
+      <c r="A40" s="4"/>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="34">
+      <c r="A41" s="4"/>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="34">
+      <c r="A42" s="4"/>
+      <c r="B42" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A36:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>